<commit_message>
uploading EER diagram and update files
</commit_message>
<xml_diff>
--- a/classSchedule.xlsx
+++ b/classSchedule.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="93" documentId="8_{3D21C413-52BD-4E1F-8BDF-85DEFA9C3EA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5185AB91-E4BD-400D-94CB-D84792969889}"/>
   <bookViews>
-    <workbookView xWindow="11508" yWindow="324" windowWidth="10680" windowHeight="12000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Class Schedule" sheetId="2" r:id="rId1"/>
@@ -452,7 +452,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
     <numFmt numFmtId="165" formatCode=";;;@"/>
-    <numFmt numFmtId="168" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -637,15 +637,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="7" applyBorder="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="7">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="6" applyFill="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -655,11 +646,20 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="9" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="5" applyNumberFormat="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="5" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="6" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="7" applyBorder="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="7">
+      <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -675,6 +675,30 @@
     <cellStyle name="Time" xfId="5" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
   </cellStyles>
   <dxfs count="28">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -861,30 +885,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -1442,25 +1442,25 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="ClassSchedule" displayName="ClassSchedule" ref="B3:I56" headerRowCellStyle="Heading 4">
   <autoFilter ref="B3:I56" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="TIME" totalsRowLabel="Total" dataDxfId="13" dataCellStyle="Time">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="TIME" totalsRowLabel="Total" dataDxfId="7" dataCellStyle="Time">
       <calculatedColumnFormula>ScheduleStart</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="SUNDAY" dataDxfId="20" dataCellStyle="Table_Details">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="SUNDAY" dataDxfId="6" dataCellStyle="Table_Details">
       <calculatedColumnFormula>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B4,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B4&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="MONDAY" dataDxfId="19" dataCellStyle="Table_Details">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="MONDAY" dataDxfId="5" dataCellStyle="Table_Details">
       <calculatedColumnFormula>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B4,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B4&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="TUESDAY" dataDxfId="18" dataCellStyle="Table_Details">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="TUESDAY" dataDxfId="4" dataCellStyle="Table_Details">
       <calculatedColumnFormula>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B4,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B4&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="WEDNESDAY" dataDxfId="17" dataCellStyle="Table_Details">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="WEDNESDAY" dataDxfId="3" dataCellStyle="Table_Details">
       <calculatedColumnFormula>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B4,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B4&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="THURSDAY" dataDxfId="16" dataCellStyle="Table_Details">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="THURSDAY" dataDxfId="2" dataCellStyle="Table_Details">
       <calculatedColumnFormula>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B4,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B4&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="FRIDAY" dataDxfId="15" dataCellStyle="Table_Details">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="FRIDAY" dataDxfId="1" dataCellStyle="Table_Details">
       <calculatedColumnFormula>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B4,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B4&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="SATURDAY" totalsRowFunction="sum" dataCellStyle="Table_Details">
@@ -1486,7 +1486,7 @@
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="LOCATION" dataCellStyle="Table_Details"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="START TIME" dataCellStyle="Time"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="END TIME" dataCellStyle="Time"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="UNIQUE" dataDxfId="14">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="UNIQUE" dataDxfId="0">
       <calculatedColumnFormula>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1732,9 +1732,7 @@
   </sheetPr>
   <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="109" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I2"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScale="109" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1748,36 +1746,36 @@
   <sheetData>
     <row r="1" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1"/>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
       <c r="G1" s="6" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="17" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
       <c r="G2" s="7">
         <v>0.33333333333333331</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="I2" s="12"/>
+      <c r="I2" s="17"/>
     </row>
     <row r="3" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
@@ -1806,8 +1804,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="17">
-        <f>ScheduleStart</f>
+      <c r="B4" s="14">
+        <f t="shared" ref="B4:B35" si="0">ScheduleStart</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="C4" s="8" t="s">
@@ -1839,11 +1837,11 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="17">
-        <f>ScheduleStart</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="C5" s="18"/>
+      <c r="B5" s="14">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C5" s="15"/>
       <c r="D5" s="8" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B5,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B5&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>CIS207</v>
@@ -1870,8 +1868,8 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="17">
-        <f>ScheduleStart</f>
+      <c r="B6" s="14">
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C6" s="8"/>
@@ -1901,8 +1899,8 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="17">
-        <f>ScheduleStart</f>
+      <c r="B7" s="14">
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C7" s="8"/>
@@ -1932,8 +1930,8 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="17">
-        <f>ScheduleStart</f>
+      <c r="B8" s="14">
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C8" s="8">
@@ -1966,8 +1964,8 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="17">
-        <f>ScheduleStart</f>
+      <c r="B9" s="14">
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C9" s="8">
@@ -2000,8 +1998,8 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="17">
-        <f>ScheduleStart</f>
+      <c r="B10" s="14">
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C10" s="8">
@@ -2034,8 +2032,8 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="17">
-        <f>ScheduleStart</f>
+      <c r="B11" s="14">
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C11" s="8">
@@ -2068,8 +2066,8 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="17">
-        <f>ScheduleStart</f>
+      <c r="B12" s="14">
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C12" s="8">
@@ -2102,8 +2100,8 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="B13" s="17">
-        <f>ScheduleStart</f>
+      <c r="B13" s="14">
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C13" s="8">
@@ -2136,8 +2134,8 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="17">
-        <f>ScheduleStart</f>
+      <c r="B14" s="14">
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C14" s="8">
@@ -2170,8 +2168,8 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="17">
-        <f>ScheduleStart</f>
+      <c r="B15" s="14">
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C15" s="8">
@@ -2205,7 +2203,7 @@
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="5">
-        <f>ScheduleStart</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C16" s="8">
@@ -2239,7 +2237,7 @@
     </row>
     <row r="17" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="5">
-        <f>ScheduleStart</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C17" s="8">
@@ -2273,7 +2271,7 @@
     </row>
     <row r="18" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="5">
-        <f>ScheduleStart</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C18" s="8">
@@ -2307,7 +2305,7 @@
     </row>
     <row r="19" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="5">
-        <f>ScheduleStart</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C19" s="8">
@@ -2341,7 +2339,7 @@
     </row>
     <row r="20" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="5">
-        <f>ScheduleStart</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C20" s="8">
@@ -2375,7 +2373,7 @@
     </row>
     <row r="21" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="5">
-        <f>ScheduleStart</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C21" s="8">
@@ -2409,7 +2407,7 @@
     </row>
     <row r="22" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="5">
-        <f>ScheduleStart</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C22" s="8">
@@ -2444,7 +2442,7 @@
     <row r="23" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23"/>
       <c r="B23" s="5">
-        <f>ScheduleStart</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C23" s="8">
@@ -2479,7 +2477,7 @@
     <row r="24" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24"/>
       <c r="B24" s="5">
-        <f>ScheduleStart</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C24" s="8">
@@ -2513,7 +2511,7 @@
     </row>
     <row r="25" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="5">
-        <f>ScheduleStart</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C25" s="8">
@@ -2547,7 +2545,7 @@
     </row>
     <row r="26" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="5">
-        <f>ScheduleStart</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C26" s="8">
@@ -2581,7 +2579,7 @@
     </row>
     <row r="27" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="5">
-        <f>ScheduleStart</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C27" s="8">
@@ -2615,7 +2613,7 @@
     </row>
     <row r="28" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="5">
-        <f>ScheduleStart</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C28" s="8">
@@ -2649,7 +2647,7 @@
     </row>
     <row r="29" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="5">
-        <f>ScheduleStart</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C29" s="8">
@@ -2683,7 +2681,7 @@
     </row>
     <row r="30" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="5">
-        <f>ScheduleStart</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C30" s="8">
@@ -2717,7 +2715,7 @@
     </row>
     <row r="31" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="5">
-        <f>ScheduleStart</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C31" s="8">
@@ -2751,7 +2749,7 @@
     </row>
     <row r="32" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="5">
-        <f>ScheduleStart</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C32" s="8">
@@ -2785,7 +2783,7 @@
     </row>
     <row r="33" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="5">
-        <f>ScheduleStart</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C33" s="8">
@@ -2819,7 +2817,7 @@
     </row>
     <row r="34" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="5">
-        <f>ScheduleStart</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C34" s="8">
@@ -2853,7 +2851,7 @@
     </row>
     <row r="35" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="5">
-        <f>ScheduleStart</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C35" s="8">
@@ -2887,7 +2885,7 @@
     </row>
     <row r="36" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="5">
-        <f>ScheduleStart</f>
+        <f t="shared" ref="B36:B56" si="1">ScheduleStart</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="C36" s="8">
@@ -2921,7 +2919,7 @@
     </row>
     <row r="37" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="5">
-        <f>ScheduleStart</f>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C37" s="8">
@@ -2955,7 +2953,7 @@
     </row>
     <row r="38" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="5">
-        <f>ScheduleStart</f>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C38" s="8">
@@ -2989,7 +2987,7 @@
     </row>
     <row r="39" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="5">
-        <f>ScheduleStart</f>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C39" s="8">
@@ -3023,7 +3021,7 @@
     </row>
     <row r="40" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="5">
-        <f>ScheduleStart</f>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C40" s="8">
@@ -3057,7 +3055,7 @@
     </row>
     <row r="41" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="5">
-        <f>ScheduleStart</f>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C41" s="8">
@@ -3091,7 +3089,7 @@
     </row>
     <row r="42" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="5">
-        <f>ScheduleStart</f>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C42" s="8">
@@ -3125,7 +3123,7 @@
     </row>
     <row r="43" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="5">
-        <f>ScheduleStart</f>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C43" s="8">
@@ -3159,7 +3157,7 @@
     </row>
     <row r="44" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="5">
-        <f>ScheduleStart</f>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C44" s="8">
@@ -3193,7 +3191,7 @@
     </row>
     <row r="45" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="5">
-        <f>ScheduleStart</f>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C45" s="8">
@@ -3227,7 +3225,7 @@
     </row>
     <row r="46" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="5">
-        <f>ScheduleStart</f>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C46" s="8">
@@ -3261,7 +3259,7 @@
     </row>
     <row r="47" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="5">
-        <f>ScheduleStart</f>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C47" s="8">
@@ -3295,7 +3293,7 @@
     </row>
     <row r="48" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="5">
-        <f>ScheduleStart</f>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C48" s="8">
@@ -3329,7 +3327,7 @@
     </row>
     <row r="49" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="5">
-        <f>ScheduleStart</f>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C49" s="8">
@@ -3363,7 +3361,7 @@
     </row>
     <row r="50" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="5">
-        <f>ScheduleStart</f>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C50" s="8">
@@ -3397,7 +3395,7 @@
     </row>
     <row r="51" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="5">
-        <f>ScheduleStart</f>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C51" s="8">
@@ -3431,7 +3429,7 @@
     </row>
     <row r="52" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="5">
-        <f>ScheduleStart</f>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C52" s="8">
@@ -3465,7 +3463,7 @@
     </row>
     <row r="53" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="5">
-        <f>ScheduleStart</f>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C53" s="8">
@@ -3499,7 +3497,7 @@
     </row>
     <row r="54" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="5">
-        <f>ScheduleStart</f>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C54" s="8">
@@ -3533,7 +3531,7 @@
     </row>
     <row r="55" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="5">
-        <f>ScheduleStart</f>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C55" s="8">
@@ -3567,7 +3565,7 @@
     </row>
     <row r="56" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="5">
-        <f>ScheduleStart</f>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C56" s="8">
@@ -3606,49 +3604,49 @@
     <mergeCell ref="I1:I2"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:I56">
-    <cfRule type="expression" dxfId="12" priority="3">
+    <cfRule type="expression" dxfId="20" priority="3">
       <formula>(C4=C3)*(C$3=ThisWeekday)*(C4&lt;&gt;0)*($B4&lt;Cal_Endtime)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="4">
+    <cfRule type="expression" dxfId="19" priority="4">
       <formula>(C$3=ThisWeekday)*(C4&lt;&gt;0)*($B4&lt;Cal_Endtime)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="7">
+    <cfRule type="expression" dxfId="18" priority="7">
       <formula>(C4=C3)*(C4&lt;&gt;0)*($B4&lt;Cal_Endtime)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="9">
+    <cfRule type="expression" dxfId="17" priority="9">
       <formula>(C4&lt;&gt;0)*($B4&lt;Cal_Endtime)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="10">
+    <cfRule type="expression" dxfId="16" priority="10">
       <formula>(C$3=ThisWeekday)*($B4&lt;Cal_Endtime)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="299">
+    <cfRule type="expression" dxfId="15" priority="299">
       <formula>C4=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:I3">
-    <cfRule type="expression" dxfId="6" priority="5">
+    <cfRule type="expression" dxfId="14" priority="5">
       <formula>(B3=ThisWeekday)*($B4&lt;Cal_Endtime)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:I56">
-    <cfRule type="expression" dxfId="5" priority="401">
+    <cfRule type="expression" dxfId="13" priority="401">
       <formula>($B4&lt;=CurrentTime)*($B5&gt;=CurrentTime)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="402">
+    <cfRule type="expression" dxfId="12" priority="402">
       <formula>(ROW(B4)&lt;ROW(INDEX($B$4:$B81,MATCH(Cal_Endtime,$B$4:$B$81,1),1))+1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="403">
+    <cfRule type="expression" dxfId="11" priority="403">
       <formula>B4=B3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="404" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="404" stopIfTrue="1">
       <formula>(B4&gt;Cal_Endtime)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="405">
+    <cfRule type="expression" dxfId="9" priority="405">
       <formula>INDEX($B$4:$B81,MATCH(Cal_Endtime,$B$4:$B$81,1),1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:C6">
-    <cfRule type="uniqueValues" dxfId="0" priority="1"/>
+    <cfRule type="uniqueValues" dxfId="8" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="16">
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a start time from the list. Select CANCEL, and then press ALT+DOWN ARROW to select start time from the drop-down list" prompt="Enter schedule start time in this cell. Press ALT+DOWN ARROW to open the drop-down list, and then press ENTER to select the time" sqref="G2" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -3697,7 +3695,7 @@
   <dimension ref="A1:H55"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D75" sqref="D75"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3713,18 +3711,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16"/>
-      <c r="B1" s="11" t="s">
+      <c r="A1" s="13"/>
+      <c r="B1" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="13" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="13"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
@@ -3942,720 +3940,720 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
       <c r="H11" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
       <c r="H12" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
       <c r="H13" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
       <c r="H14" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
       <c r="H15" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
       <c r="H16" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
       <c r="H17" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
       <c r="H18" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>16</v>
       </c>
     </row>
     <row r="19" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
       <c r="H19" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>17</v>
       </c>
     </row>
     <row r="20" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
       <c r="H20" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>18</v>
       </c>
     </row>
     <row r="21" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
       <c r="H21" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>19</v>
       </c>
     </row>
     <row r="22" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
       <c r="H22" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>20</v>
       </c>
     </row>
     <row r="23" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
       <c r="H23" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>21</v>
       </c>
     </row>
     <row r="24" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
       <c r="H24" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>22</v>
       </c>
     </row>
     <row r="25" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
       <c r="H25" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>23</v>
       </c>
     </row>
     <row r="26" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
       <c r="H26" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>24</v>
       </c>
     </row>
     <row r="27" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
       <c r="H27" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>25</v>
       </c>
     </row>
     <row r="28" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
       <c r="H28" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>26</v>
       </c>
     </row>
     <row r="29" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C29" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
       <c r="H29" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>27</v>
       </c>
     </row>
     <row r="30" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
       <c r="H30" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>28</v>
       </c>
     </row>
     <row r="31" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="14" t="s">
+      <c r="B31" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
       <c r="H31" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>29</v>
       </c>
     </row>
     <row r="32" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
       <c r="H32" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>30</v>
       </c>
     </row>
     <row r="33" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="14" t="s">
+      <c r="B33" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C33" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
       <c r="H33" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>31</v>
       </c>
     </row>
     <row r="34" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="15"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
       <c r="H34" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>32</v>
       </c>
     </row>
     <row r="35" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="14" t="s">
+      <c r="B35" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="C35" s="14" t="s">
+      <c r="C35" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="15"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
       <c r="H35" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>33</v>
       </c>
     </row>
     <row r="36" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="14" t="s">
+      <c r="B36" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="C36" s="14" t="s">
+      <c r="C36" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="15"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
       <c r="H36" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>34</v>
       </c>
     </row>
     <row r="37" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="14" t="s">
+      <c r="B37" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="C37" s="14" t="s">
+      <c r="C37" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="15"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
       <c r="H37" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>35</v>
       </c>
     </row>
     <row r="38" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="14" t="s">
+      <c r="B38" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="C38" s="14" t="s">
+      <c r="C38" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
       <c r="H38" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>36</v>
       </c>
     </row>
     <row r="39" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="14" t="s">
+      <c r="B39" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="C39" s="14" t="s">
+      <c r="C39" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="15"/>
-      <c r="G39" s="15"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
       <c r="H39" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>37</v>
       </c>
     </row>
     <row r="40" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="14" t="s">
+      <c r="B40" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="C40" s="14" t="s">
+      <c r="C40" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="15"/>
-      <c r="G40" s="15"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
       <c r="H40" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>38</v>
       </c>
     </row>
     <row r="41" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="14" t="s">
+      <c r="B41" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="C41" s="14" t="s">
+      <c r="C41" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="15"/>
-      <c r="G41" s="15"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="12"/>
       <c r="H41" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>39</v>
       </c>
     </row>
     <row r="42" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="14" t="s">
+      <c r="B42" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="C42" s="14" t="s">
+      <c r="C42" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="15"/>
-      <c r="G42" s="15"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
       <c r="H42" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>40</v>
       </c>
     </row>
     <row r="43" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="14" t="s">
+      <c r="B43" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="C43" s="14" t="s">
+      <c r="C43" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="15"/>
-      <c r="G43" s="15"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="12"/>
       <c r="H43" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>41</v>
       </c>
     </row>
     <row r="44" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="14" t="s">
+      <c r="B44" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="C44" s="14" t="s">
+      <c r="C44" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="D44" s="14"/>
-      <c r="E44" s="14"/>
-      <c r="F44" s="15"/>
-      <c r="G44" s="15"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
       <c r="H44" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>42</v>
       </c>
     </row>
     <row r="45" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="14" t="s">
+      <c r="B45" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="C45" s="14" t="s">
+      <c r="C45" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="D45" s="14"/>
-      <c r="E45" s="14"/>
-      <c r="F45" s="15"/>
-      <c r="G45" s="15"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
       <c r="H45" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>43</v>
       </c>
     </row>
     <row r="46" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="14" t="s">
+      <c r="B46" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="C46" s="14" t="s">
+      <c r="C46" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="D46" s="14"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="15"/>
-      <c r="G46" s="15"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12"/>
       <c r="H46" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>44</v>
       </c>
     </row>
     <row r="47" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="14" t="s">
+      <c r="B47" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="C47" s="14" t="s">
+      <c r="C47" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="15"/>
-      <c r="G47" s="15"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="12"/>
+      <c r="G47" s="12"/>
       <c r="H47" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>45</v>
       </c>
     </row>
     <row r="48" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="14" t="s">
+      <c r="B48" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="C48" s="14" t="s">
+      <c r="C48" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="15"/>
-      <c r="G48" s="15"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="12"/>
       <c r="H48" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>46</v>
       </c>
     </row>
     <row r="49" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="14" t="s">
+      <c r="B49" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="C49" s="14" t="s">
+      <c r="C49" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="15"/>
-      <c r="G49" s="15"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
       <c r="H49" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>47</v>
       </c>
     </row>
     <row r="50" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="14" t="s">
+      <c r="B50" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="C50" s="14" t="s">
+      <c r="C50" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="15"/>
-      <c r="G50" s="15"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="12"/>
+      <c r="G50" s="12"/>
       <c r="H50" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>48</v>
       </c>
     </row>
     <row r="51" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="14" t="s">
+      <c r="B51" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="C51" s="14" t="s">
+      <c r="C51" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="D51" s="14"/>
-      <c r="E51" s="14"/>
-      <c r="F51" s="15"/>
-      <c r="G51" s="15"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="12"/>
+      <c r="G51" s="12"/>
       <c r="H51" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>49</v>
       </c>
     </row>
     <row r="52" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="14" t="s">
+      <c r="B52" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="C52" s="14" t="s">
+      <c r="C52" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="15"/>
-      <c r="G52" s="15"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="11"/>
+      <c r="F52" s="12"/>
+      <c r="G52" s="12"/>
       <c r="H52" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>50</v>
       </c>
     </row>
     <row r="53" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="14" t="s">
+      <c r="B53" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="C53" s="14" t="s">
+      <c r="C53" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="D53" s="14"/>
-      <c r="E53" s="14"/>
-      <c r="F53" s="15"/>
-      <c r="G53" s="15"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="11"/>
+      <c r="F53" s="12"/>
+      <c r="G53" s="12"/>
       <c r="H53" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>51</v>
       </c>
     </row>
     <row r="54" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="14" t="s">
+      <c r="B54" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="C54" s="14" t="s">
+      <c r="C54" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="D54" s="14"/>
-      <c r="E54" s="14"/>
-      <c r="F54" s="15"/>
-      <c r="G54" s="15"/>
+      <c r="D54" s="11"/>
+      <c r="E54" s="11"/>
+      <c r="F54" s="12"/>
+      <c r="G54" s="12"/>
       <c r="H54" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>52</v>
       </c>
     </row>
     <row r="55" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="14" t="s">
+      <c r="B55" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="C55" s="14" t="s">
+      <c r="C55" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="D55" s="14"/>
-      <c r="E55" s="14"/>
-      <c r="F55" s="15"/>
-      <c r="G55" s="15"/>
+      <c r="D55" s="11"/>
+      <c r="E55" s="11"/>
+      <c r="F55" s="12"/>
+      <c r="G55" s="12"/>
       <c r="H55" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>53</v>

</xml_diff>